<commit_message>
add a readme with all info about the data
</commit_message>
<xml_diff>
--- a/zhang_ma/research availability_11597hours.xlsx
+++ b/zhang_ma/research availability_11597hours.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pei/Documents/credit data and data analysis 2021spring/open science framework/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schebolu\procrastination\procrastination_data\zhang_ma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0E201B-A86E-274E-8A63-E84E9835D69F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48029FCD-2865-4F73-A944-DF64AA64270D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1380" windowWidth="28800" windowHeight="13040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study_summary_report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -34,9 +34,6 @@
     <t>Participated</t>
   </si>
   <si>
-    <t>Free Spaces</t>
-  </si>
-  <si>
     <t>Credits Granted</t>
   </si>
   <si>
@@ -53,6 +50,9 @@
   </si>
   <si>
     <t>Study name index</t>
+  </si>
+  <si>
+    <t>Free Spaces (left)</t>
   </si>
 </sst>
 </file>
@@ -869,21 +869,21 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -898,21 +898,21 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1.5</v>
@@ -934,12 +934,12 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -961,12 +961,12 @@
         <v>195.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>0.5</v>
@@ -988,12 +988,12 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>0.5</v>
@@ -1015,12 +1015,12 @@
         <v>393.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1042,12 +1042,12 @@
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1069,12 +1069,12 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1096,12 +1096,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1123,12 +1123,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1150,12 +1150,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1177,12 +1177,12 @@
         <v>819</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1204,12 +1204,12 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>0.5</v>
@@ -1231,12 +1231,12 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1258,12 +1258,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1285,12 +1285,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1312,12 +1312,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1339,12 +1339,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>0.5</v>
@@ -1366,12 +1366,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>0.5</v>
@@ -1393,12 +1393,12 @@
         <v>115.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1420,12 +1420,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1447,12 +1447,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22">
         <v>0.5</v>
@@ -1474,12 +1474,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23">
         <v>0.5</v>
@@ -1501,12 +1501,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24">
         <v>0.5</v>
@@ -1528,12 +1528,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25">
         <v>0.5</v>
@@ -1555,12 +1555,12 @@
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26">
         <v>0.5</v>
@@ -1582,12 +1582,12 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27">
         <v>0.5</v>
@@ -1609,12 +1609,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28">
         <v>0.5</v>
@@ -1636,12 +1636,12 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>1.5</v>
@@ -1663,12 +1663,12 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30">
         <v>0.5</v>
@@ -1690,12 +1690,12 @@
         <v>85.5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31">
         <v>0.5</v>
@@ -1717,12 +1717,12 @@
         <v>168.5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32">
         <v>0.5</v>
@@ -1744,12 +1744,12 @@
         <v>207.5</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1771,12 +1771,12 @@
         <v>600</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -1798,12 +1798,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35">
         <v>0.5</v>
@@ -1825,12 +1825,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36">
         <v>0.5</v>
@@ -1852,12 +1852,12 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37">
         <v>0.5</v>
@@ -1879,12 +1879,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1906,12 +1906,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1933,12 +1933,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40">
         <v>0.5</v>
@@ -1960,12 +1960,12 @@
         <v>172.5</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41">
         <v>0.5</v>
@@ -1987,12 +1987,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42">
         <v>0.5</v>
@@ -2014,12 +2014,12 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43">
         <v>0.5</v>
@@ -2041,12 +2041,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C44">
         <v>0.5</v>
@@ -2068,12 +2068,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C45">
         <v>0.5</v>
@@ -2095,12 +2095,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46">
         <v>0.5</v>
@@ -2122,12 +2122,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47">
         <v>0.5</v>
@@ -2149,12 +2149,12 @@
         <v>443</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C48">
         <v>0.5</v>
@@ -2176,12 +2176,12 @@
         <v>397.5</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C49">
         <v>0.5</v>
@@ -2203,12 +2203,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2230,12 +2230,12 @@
         <v>745</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51">
         <v>0.5</v>
@@ -2257,12 +2257,12 @@
         <v>342.5</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52">
         <v>0.5</v>
@@ -2284,12 +2284,12 @@
         <v>191.5</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53">
         <v>0.5</v>
@@ -2311,12 +2311,12 @@
         <v>257.5</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54">
         <v>0.5</v>
@@ -2338,12 +2338,12 @@
         <v>144.5</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C55">
         <v>0.5</v>
@@ -2365,12 +2365,12 @@
         <v>99.5</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -2392,12 +2392,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -2419,9 +2419,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E58">
         <v>9933</v>

</xml_diff>

<commit_message>
try out some models based on discounting and efficacy to get time course patterns
</commit_message>
<xml_diff>
--- a/zhang_ma/research availability_11597hours.xlsx
+++ b/zhang_ma/research availability_11597hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schebolu\procrastination\procrastination_data\zhang_ma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48029FCD-2865-4F73-A944-DF64AA64270D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF05423E-B2B5-4260-8095-FCB1E751125F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study_summary_report" sheetId="1" r:id="rId1"/>

</xml_diff>